<commit_message>
MENT-213: Create Questions Category on the webApp
</commit_message>
<xml_diff>
--- a/mentoring-core/add-health-facilities_20181029.xlsx
+++ b/mentoring-core/add-health-facilities_20181029.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steliomo/workspace/mentoring/mentoring-core/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09567E2D-2DE2-B94E-BE7A-F47A5593C66D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62818539-2F9A-8149-A792-E24DDCCBF552}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="107">
   <si>
     <t>CS Malua</t>
   </si>
@@ -329,6 +329,18 @@
   </si>
   <si>
     <t>PS Munhiba</t>
+  </si>
+  <si>
+    <t>Pebane</t>
+  </si>
+  <si>
+    <t>PS Cutal</t>
+  </si>
+  <si>
+    <t>Namacurra</t>
+  </si>
+  <si>
+    <t>PS Naciaia</t>
   </si>
 </sst>
 </file>
@@ -698,10 +710,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:D94"/>
+  <dimension ref="B2:D96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D93" sqref="D93"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="D84" sqref="D84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1734,6 +1746,28 @@
         <v>102</v>
       </c>
     </row>
+    <row r="95" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B95" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C95" t="s">
+        <v>103</v>
+      </c>
+      <c r="D95" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="96" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B96" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C96" t="s">
+        <v>105</v>
+      </c>
+      <c r="D96" t="s">
+        <v>106</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>